<commit_message>
try to allow more links by replacing ' ' with '\n'
</commit_message>
<xml_diff>
--- a/sendEmail.xlsx
+++ b/sendEmail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\school\攝影\bulk-email-sender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627BD0D4-0FBC-42F1-9758-511CBFF44DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856E3371-F1D8-4946-B9DB-4D178A0A2D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2952" windowWidth="23040" windowHeight="8892" xr2:uid="{877CC756-8061-44ED-98D8-D26C4B86854F}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>alice@example.com</t>
   </si>
   <si>
-    <t>https://example,com</t>
-  </si>
-  <si>
     <t>bob</t>
   </si>
   <si>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>https://example.org</t>
+  </si>
+  <si>
+    <t>https://example.com https://google.com</t>
   </si>
 </sst>
 </file>
@@ -437,13 +437,13 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -465,35 +465,35 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{6D00F2EB-5B96-46CB-BB4B-AB712649F01D}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{DB7043EA-885E-4EA1-931E-0232B5C09279}"/>
+    <hyperlink ref="C2" r:id="rId2" display="https://example.com" xr:uid="{DB7043EA-885E-4EA1-931E-0232B5C09279}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{FCBC802C-ACFD-402B-9EFA-77FADDC7123E}"/>
     <hyperlink ref="C3" r:id="rId4" xr:uid="{5BCFADC7-3F3E-44E9-98D5-2D291469B8F8}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{9289A447-9F45-4C97-8EF0-5AA02DFFF413}"/>

</xml_diff>